<commit_message>
Improved enroll students + updated points
</commit_message>
<xml_diff>
--- a/group_info/points.xlsx
+++ b/group_info/points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GroupA_SE2_2019\group_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBB13E7-0411-41AC-8BC8-B76076723882}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC551E7B-1044-4BDC-B185-15C1C04A301E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -441,7 +441,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +486,7 @@
       </c>
       <c r="D3" s="5">
         <f>SUM(B3:B14)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
@@ -510,8 +510,12 @@
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="3">
+        <v>43784</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5</v>
+      </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>

</xml_diff>

<commit_message>
Added persona + updated points
</commit_message>
<xml_diff>
--- a/group_info/points.xlsx
+++ b/group_info/points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GroupA_SE2_2019\group_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31464CD2-20BB-44B9-A414-5F06861588F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BBA8AC-90D1-46C2-B3A8-2A9FB202E788}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -267,8 +267,14 @@
                 <c:pt idx="4">
                   <c:v>43784</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>43788</c:v>
+                <c:pt idx="5">
+                  <c:v>43785</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43786</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43787</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -298,13 +304,10 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -364,7 +367,7 @@
                   <c:v>43774</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43788</c:v>
+                  <c:v>43787</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1435,8 +1438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,7 +1524,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="3">
-        <v>43788</v>
+        <v>43787</v>
       </c>
       <c r="D4" s="4">
         <v>34</v>
@@ -1596,6 +1599,9 @@
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>43785</v>
+      </c>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1610,49 +1616,48 @@
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="3">
+        <v>43786</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="F9" s="5">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>43787</v>
+      </c>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="F10" s="5">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>43788</v>
-      </c>
+      <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="F11" s="5">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="G11" s="5">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>

</xml_diff>

<commit_message>
Updated points + sidebar CSS improved
</commit_message>
<xml_diff>
--- a/group_info/points.xlsx
+++ b/group_info/points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GroupA_SE2_2019\group_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BBA8AC-90D1-46C2-B3A8-2A9FB202E788}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D304AFF-EFB5-4016-99D4-4818BD58417A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Estimated points left</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
   </si>
 </sst>
 </file>
@@ -1134,16 +1137,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>91588</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1781175</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>229819</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1436,10 +1439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,6 +1464,10 @@
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1534,7 +1541,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="5">
-        <f t="shared" ref="G4:G11" si="0">$E$3-F4</f>
+        <f t="shared" ref="G4:G10" si="0">$E$3-F4</f>
         <v>29</v>
       </c>
       <c r="H4" s="5">
@@ -1551,7 +1558,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="F5" s="5">
-        <f t="shared" ref="F5:F11" si="1">B5+F4</f>
+        <f t="shared" ref="F5:F10" si="1">B5+F4</f>
         <v>8</v>
       </c>
       <c r="G5" s="5">
@@ -1677,15 +1684,296 @@
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+    <row r="15" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>43789</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3">
+        <v>43789</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5">
+        <v>34</v>
+      </c>
+      <c r="F17" s="5">
+        <f>B17</f>
+        <v>1</v>
+      </c>
+      <c r="G17" s="5">
+        <f>$E$3-F17</f>
+        <v>33</v>
+      </c>
+      <c r="H17" s="5">
+        <f>D18</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>43790</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3">
+        <v>43772</v>
+      </c>
+      <c r="D18" s="4">
+        <f>E17</f>
+        <v>34</v>
+      </c>
+      <c r="F18" s="5">
+        <f>B18+F17</f>
+        <v>1</v>
+      </c>
+      <c r="G18" s="5">
+        <f t="shared" ref="G18:G30" si="2">$E$3-F18</f>
+        <v>33</v>
+      </c>
+      <c r="H18" s="5">
+        <f>D17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>43791</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="F19" s="5">
+        <f t="shared" ref="F19:F30" si="3">B19+F18</f>
+        <v>1</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>43792</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="F20" s="5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G20" s="5">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>43793</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="F21" s="5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>43794</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="F22" s="5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G22" s="5">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>43795</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="F23" s="5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G23" s="5">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>43796</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="F24" s="5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G24" s="5">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>43797</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="F25" s="5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G25" s="5">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>43798</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="F26" s="5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G26" s="5">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>43799</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="F27" s="5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G27" s="5">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>43800</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="F28" s="5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G28" s="5">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>43801</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="F29" s="5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G29" s="5">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>43802</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="F30" s="5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G30" s="5">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A15:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Coursepage + courselist updated
</commit_message>
<xml_diff>
--- a/group_info/points.xlsx
+++ b/group_info/points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GroupA_SE2_2019\group_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D304AFF-EFB5-4016-99D4-4818BD58417A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C8C278-830C-4D31-BD48-853F218B900D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -52,6 +54,9 @@
   </si>
   <si>
     <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Target</t>
   </si>
 </sst>
 </file>
@@ -1441,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,7 +1760,9 @@
       <c r="A18" s="3">
         <v>43790</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="4">
+        <v>0</v>
+      </c>
       <c r="C18" s="3">
         <v>43772</v>
       </c>
@@ -1780,7 +1787,9 @@
       <c r="A19" s="3">
         <v>43791</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="4">
+        <v>0</v>
+      </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="F19" s="5">
@@ -1793,11 +1802,13 @@
       </c>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>43792</v>
       </c>
-      <c r="B20" s="4"/>
+      <c r="B20" s="4">
+        <v>0</v>
+      </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="F20" s="5">
@@ -1808,13 +1819,17 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="H20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>43793</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="4">
+        <v>0</v>
+      </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="F21" s="5">
@@ -1825,13 +1840,17 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="H21" s="5"/>
+      <c r="H21" s="5">
+        <v>21</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>43794</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="4">
+        <v>0</v>
+      </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="F22" s="5">
@@ -1842,13 +1861,17 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="H22" s="5"/>
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>43795</v>
       </c>
-      <c r="B23" s="4"/>
+      <c r="B23" s="4">
+        <v>0</v>
+      </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="F23" s="5">
@@ -1865,7 +1888,9 @@
       <c r="A24" s="3">
         <v>43796</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4">
+        <v>0</v>
+      </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="F24" s="5">
@@ -1882,7 +1907,9 @@
       <c r="A25" s="3">
         <v>43797</v>
       </c>
-      <c r="B25" s="4"/>
+      <c r="B25" s="4">
+        <v>0</v>
+      </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="F25" s="5">
@@ -1898,7 +1925,9 @@
       <c r="A26" s="3">
         <v>43798</v>
       </c>
-      <c r="B26" s="4"/>
+      <c r="B26" s="4">
+        <v>0</v>
+      </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="F26" s="5">
@@ -1914,16 +1943,18 @@
       <c r="A27" s="3">
         <v>43799</v>
       </c>
-      <c r="B27" s="4"/>
+      <c r="B27" s="4">
+        <v>4</v>
+      </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="F27" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G27" s="5">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -1935,11 +1966,11 @@
       <c r="D28" s="5"/>
       <c r="F28" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G28" s="5">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -1949,11 +1980,11 @@
       <c r="B29" s="4"/>
       <c r="F29" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G29" s="5">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -1963,11 +1994,11 @@
       <c r="B30" s="4"/>
       <c r="F30" s="5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G30" s="5">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated points + improved courselist
</commit_message>
<xml_diff>
--- a/group_info/points.xlsx
+++ b/group_info/points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GroupA_SE2_2019\group_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0C650F-3932-4F97-9F10-FE30102CCFB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA18B7C-872F-488C-969C-00E6E8B84639}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,6 +396,372 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-ACA6-4BD9-BF68-884F99FBBE04}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="813059824"/>
+        <c:axId val="635105824"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="813059824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="635105824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="635105824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="813059824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.9228535923455425E-2"/>
+          <c:y val="7.3732711759477321E-2"/>
+          <c:w val="0.90738864648288386"/>
+          <c:h val="0.86925158201177288"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Points left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$21:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>43789</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$E$21:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E25-4677-AB5F-D454AA0AD107}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimated points left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$C$17:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43789</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43802</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$H$17:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7E25-4677-AB5F-D454AA0AD107}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -619,7 +985,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1170,6 +2092,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>276225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>223679</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Grafico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D54E3B1B-2CBF-427F-AC7B-0E49D04EA63D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1443,8 +2403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,19 +2698,19 @@
         <v>0</v>
       </c>
       <c r="E17" s="5">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F17" s="5">
         <f>B17</f>
         <v>1</v>
       </c>
       <c r="G17" s="5">
-        <f>$E$3-F17</f>
-        <v>33</v>
+        <f>$E$17-F17</f>
+        <v>21</v>
       </c>
       <c r="H17" s="5">
         <f>D18</f>
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -1761,19 +2721,19 @@
         <v>0</v>
       </c>
       <c r="C18" s="3">
-        <v>43772</v>
+        <v>43802</v>
       </c>
       <c r="D18" s="4">
         <f>E17</f>
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F18" s="5">
         <f>B18+F17</f>
         <v>1</v>
       </c>
       <c r="G18" s="5">
-        <f t="shared" ref="G18:G30" si="2">$E$3-F18</f>
-        <v>33</v>
+        <f t="shared" ref="G18:G30" si="2">$E$17-F18</f>
+        <v>21</v>
       </c>
       <c r="H18" s="5">
         <f>D17</f>
@@ -1795,7 +2755,7 @@
       </c>
       <c r="G19" s="5">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="H19" s="5"/>
     </row>
@@ -1814,7 +2774,7 @@
       </c>
       <c r="G20" s="5">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="H20" s="5"/>
     </row>
@@ -1826,14 +2786,20 @@
         <v>0</v>
       </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="D21" s="3">
+        <v>43789</v>
+      </c>
+      <c r="E21" s="4">
+        <f>G17</f>
+        <v>21</v>
+      </c>
       <c r="F21" s="5">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G21" s="5">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="H21" s="5"/>
     </row>
@@ -1845,14 +2811,20 @@
         <v>0</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+      <c r="D22" s="3">
+        <v>43799</v>
+      </c>
+      <c r="E22" s="4">
+        <f>G27</f>
+        <v>16</v>
+      </c>
       <c r="F22" s="5">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G22" s="5">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="H22" s="5"/>
     </row>
@@ -1864,14 +2836,20 @@
         <v>0</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="D23" s="3">
+        <v>43801</v>
+      </c>
+      <c r="E23" s="4">
+        <f>G29</f>
+        <v>11</v>
+      </c>
       <c r="F23" s="5">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G23" s="5">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="H23" s="5"/>
     </row>
@@ -1890,7 +2868,7 @@
       </c>
       <c r="G24" s="5">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="H24" s="5"/>
     </row>
@@ -1909,7 +2887,7 @@
       </c>
       <c r="G25" s="5">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -1927,7 +2905,7 @@
       </c>
       <c r="G26" s="5">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -1945,14 +2923,16 @@
       </c>
       <c r="G27" s="5">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>43800</v>
       </c>
-      <c r="B28" s="4"/>
+      <c r="B28" s="4">
+        <v>0</v>
+      </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="F28" s="5">
@@ -1961,21 +2941,23 @@
       </c>
       <c r="G28" s="5">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>43801</v>
       </c>
-      <c r="B29" s="4"/>
+      <c r="B29" s="4">
+        <v>5</v>
+      </c>
       <c r="F29" s="5">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G29" s="5">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -1985,11 +2967,11 @@
       <c r="B30" s="4"/>
       <c r="F30" s="5">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G30" s="5">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated points + fixed sidebar
</commit_message>
<xml_diff>
--- a/group_info/points.xlsx
+++ b/group_info/points.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GroupA_SE2_2019\group_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960E39A0-FF79-49F6-A2AA-5F7B5347EEA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF716824-1F51-438D-B170-A80886E7CA7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2418,8 +2418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3174,18 +3174,18 @@
         <v>43809</v>
       </c>
       <c r="B40" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="7"/>
       <c r="E40" s="8"/>
       <c r="F40" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G40" s="5">
         <f t="shared" si="4"/>
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H40" s="5"/>
     </row>
@@ -3201,11 +3201,11 @@
       <c r="E41" s="8"/>
       <c r="F41" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G41" s="5">
         <f t="shared" si="4"/>
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H41" s="5"/>
     </row>
@@ -3220,11 +3220,11 @@
       <c r="D42" s="5"/>
       <c r="F42" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G42" s="5">
         <f t="shared" si="4"/>
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -3238,11 +3238,11 @@
       <c r="D43" s="5"/>
       <c r="F43" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G43" s="5">
         <f t="shared" si="4"/>
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -3256,11 +3256,11 @@
       <c r="D44" s="5"/>
       <c r="F44" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G44" s="5">
         <f t="shared" si="4"/>
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -3274,11 +3274,11 @@
       <c r="D45" s="5"/>
       <c r="F45" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G45" s="5">
         <f t="shared" si="4"/>
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -3290,11 +3290,11 @@
       </c>
       <c r="F46" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G46" s="5">
         <f t="shared" si="4"/>
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -3306,11 +3306,11 @@
       </c>
       <c r="F47" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G47" s="5">
         <f t="shared" si="4"/>
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed SQ bugs + updated points
</commit_message>
<xml_diff>
--- a/group_info/points.xlsx
+++ b/group_info/points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GroupA_SE2_2019\group_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF716824-1F51-438D-B170-A80886E7CA7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6ED916-1A57-4FB2-8DE4-C6CDA76F39CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2850" yWindow="2850" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -2418,7 +2418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
@@ -3174,18 +3174,18 @@
         <v>43809</v>
       </c>
       <c r="B40" s="4">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="7"/>
       <c r="E40" s="8"/>
       <c r="F40" s="5">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G40" s="5">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="H40" s="5"/>
     </row>
@@ -3201,11 +3201,11 @@
       <c r="E41" s="8"/>
       <c r="F41" s="5">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G41" s="5">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="H41" s="5"/>
     </row>
@@ -3220,11 +3220,11 @@
       <c r="D42" s="5"/>
       <c r="F42" s="5">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G42" s="5">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -3238,11 +3238,11 @@
       <c r="D43" s="5"/>
       <c r="F43" s="5">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G43" s="5">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -3256,11 +3256,11 @@
       <c r="D44" s="5"/>
       <c r="F44" s="5">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G44" s="5">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -3274,11 +3274,11 @@
       <c r="D45" s="5"/>
       <c r="F45" s="5">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G45" s="5">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -3290,11 +3290,11 @@
       </c>
       <c r="F46" s="5">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G46" s="5">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -3306,11 +3306,11 @@
       </c>
       <c r="F47" s="5">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G47" s="5">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated points + bugfix
</commit_message>
<xml_diff>
--- a/group_info/points.xlsx
+++ b/group_info/points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GroupA_SE2_2019\group_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6ED916-1A57-4FB2-8DE4-C6CDA76F39CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079AE31A-5AF2-479E-B006-72F068BA6211}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="2850" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -2419,7 +2419,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3232,17 +3232,17 @@
         <v>43812</v>
       </c>
       <c r="B43" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="F43" s="5">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G43" s="5">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -3256,11 +3256,11 @@
       <c r="D44" s="5"/>
       <c r="F44" s="5">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G44" s="5">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -3274,11 +3274,11 @@
       <c r="D45" s="5"/>
       <c r="F45" s="5">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G45" s="5">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -3290,11 +3290,11 @@
       </c>
       <c r="F46" s="5">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G46" s="5">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -3306,11 +3306,11 @@
       </c>
       <c r="F47" s="5">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G47" s="5">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated points + single student fix
</commit_message>
<xml_diff>
--- a/group_info/points.xlsx
+++ b/group_info/points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GroupA_SE2_2019\group_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079AE31A-5AF2-479E-B006-72F068BA6211}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E91AEE-2CFC-42B8-BE5E-563CFD324179}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="9">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>7 stories + 1 setup</t>
   </si>
 </sst>
 </file>
@@ -777,6 +780,392 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7E25-4677-AB5F-D454AA0AD107}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="813059824"/>
+        <c:axId val="635105824"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="813059824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="635105824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="635105824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="813059824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.9228535923455425E-2"/>
+          <c:y val="7.3732711759477321E-2"/>
+          <c:w val="0.90738864648288386"/>
+          <c:h val="0.86925158201177288"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Points left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$39:$D$42</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>43803</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43809</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43812</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43815</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$E$39:$E$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-925E-40BE-B9F5-9D29BF1F9F9E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimated points left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$C$34:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>43803</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43816</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$H$34:$H$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-925E-40BE-B9F5-9D29BF1F9F9E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1040,6 +1429,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1557,6 +1986,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2145,6 +3090,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1771650</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>14129</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Grafico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2186E32D-65FE-437F-8B2F-DA7596AC3A83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2418,8 +3401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3157,8 +4140,13 @@
         <v>0</v>
       </c>
       <c r="C39" s="5"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="8"/>
+      <c r="D39" s="3">
+        <v>43803</v>
+      </c>
+      <c r="E39" s="5">
+        <f>G34</f>
+        <v>47</v>
+      </c>
       <c r="F39" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3176,9 +4164,16 @@
       <c r="B40" s="4">
         <v>15</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="8"/>
+      <c r="C40" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="3">
+        <v>43809</v>
+      </c>
+      <c r="E40" s="4">
+        <f>G40</f>
+        <v>32</v>
+      </c>
       <c r="F40" s="5">
         <f t="shared" si="5"/>
         <v>15</v>
@@ -3197,8 +4192,13 @@
         <v>0</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="8"/>
+      <c r="D41" s="3">
+        <v>43812</v>
+      </c>
+      <c r="E41" s="4">
+        <f>G43</f>
+        <v>27</v>
+      </c>
       <c r="F41" s="5">
         <f t="shared" si="5"/>
         <v>15</v>
@@ -3217,7 +4217,13 @@
         <v>0</v>
       </c>
       <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="D42" s="3">
+        <v>43815</v>
+      </c>
+      <c r="E42" s="4">
+        <f>G46</f>
+        <v>25</v>
+      </c>
       <c r="F42" s="5">
         <f t="shared" si="5"/>
         <v>15</v>
@@ -3286,15 +4292,15 @@
         <v>43815</v>
       </c>
       <c r="B46" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F46" s="5">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G46" s="5">
         <f t="shared" si="4"/>
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -3306,11 +4312,11 @@
       </c>
       <c r="F47" s="5">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G47" s="5">
         <f t="shared" si="4"/>
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated excel + GOD FORGIVE US FOR WE HAVE BAD CODE
</commit_message>
<xml_diff>
--- a/group_info/points.xlsx
+++ b/group_info/points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GroupA_SE2_2019\group_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0067EF-ED47-4344-920E-124272D70867}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E11F3E7-BAE3-446B-B474-9E74F58B11F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1074,7 +1074,7 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3408,7 +3408,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4072,7 +4072,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="5">
-        <f t="shared" ref="E35:G47" si="4">$E$34-F35</f>
+        <f t="shared" ref="G35:G47" si="4">$E$34-F35</f>
         <v>47</v>
       </c>
       <c r="H35" s="5">
@@ -4252,7 +4252,7 @@
       </c>
       <c r="E43" s="5">
         <f>G47</f>
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F43" s="5">
         <f t="shared" si="5"/>
@@ -4320,15 +4320,15 @@
         <v>43816</v>
       </c>
       <c r="B47" s="4">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F47" s="5">
         <f t="shared" si="5"/>
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="G47" s="5">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Separated creation and population of db + docker is interactive now
</commit_message>
<xml_diff>
--- a/group_info/points.xlsx
+++ b/group_info/points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GroupA_SE2_2019\group_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E11F3E7-BAE3-446B-B474-9E74F58B11F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84115A68-7A30-4297-8E60-CA4E7F24D879}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="11">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>7 stories + 1 setup</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>13 stories + 1 setup</t>
   </si>
 </sst>
 </file>
@@ -3405,10 +3411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4331,11 +4337,560 @@
         <v>12</v>
       </c>
     </row>
+    <row r="49" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A49" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+    </row>
+    <row r="50" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>43817</v>
+      </c>
+      <c r="B51" s="4">
+        <v>0</v>
+      </c>
+      <c r="C51" s="3">
+        <v>43803</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0</v>
+      </c>
+      <c r="E51" s="5">
+        <v>55</v>
+      </c>
+      <c r="F51" s="5">
+        <f>B51</f>
+        <v>0</v>
+      </c>
+      <c r="G51" s="5">
+        <f>$E$51-F51</f>
+        <v>55</v>
+      </c>
+      <c r="H51" s="5">
+        <f>D52</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>43818</v>
+      </c>
+      <c r="B52" s="4">
+        <v>0</v>
+      </c>
+      <c r="C52" s="3">
+        <v>43816</v>
+      </c>
+      <c r="D52" s="4">
+        <f>E51</f>
+        <v>55</v>
+      </c>
+      <c r="F52" s="5">
+        <f>B52+F51</f>
+        <v>0</v>
+      </c>
+      <c r="G52" s="5">
+        <f t="shared" ref="G52:G78" si="6">$E$51-F52</f>
+        <v>55</v>
+      </c>
+      <c r="H52" s="5">
+        <f>D51</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>43819</v>
+      </c>
+      <c r="B53" s="4">
+        <v>15</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="F53" s="5">
+        <f t="shared" ref="F53:F78" si="7">B53+F52</f>
+        <v>15</v>
+      </c>
+      <c r="G53" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>43820</v>
+      </c>
+      <c r="B54" s="4">
+        <v>0</v>
+      </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="F54" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G54" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>43821</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G55" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>43822</v>
+      </c>
+      <c r="B56" s="4">
+        <v>0</v>
+      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" s="3">
+        <v>43819</v>
+      </c>
+      <c r="E56" s="4">
+        <v>15</v>
+      </c>
+      <c r="F56" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G56" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>43823</v>
+      </c>
+      <c r="B57" s="4">
+        <v>0</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="7"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G57" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="H57" s="5"/>
+    </row>
+    <row r="58" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>43824</v>
+      </c>
+      <c r="B58" s="4">
+        <v>0</v>
+      </c>
+      <c r="C58" s="5"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G58" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>43825</v>
+      </c>
+      <c r="B59" s="4">
+        <v>0</v>
+      </c>
+      <c r="C59" s="5"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G59" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>43826</v>
+      </c>
+      <c r="B60" s="4">
+        <v>0</v>
+      </c>
+      <c r="C60" s="5"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G60" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>43827</v>
+      </c>
+      <c r="B61" s="4">
+        <v>0</v>
+      </c>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="F61" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G61" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>43828</v>
+      </c>
+      <c r="B62" s="4">
+        <v>0</v>
+      </c>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="F62" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G62" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>43829</v>
+      </c>
+      <c r="B63" s="4">
+        <v>0</v>
+      </c>
+      <c r="F63" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G63" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <v>43830</v>
+      </c>
+      <c r="B64" s="4">
+        <v>0</v>
+      </c>
+      <c r="F64" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G64" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
+        <v>43831</v>
+      </c>
+      <c r="B65" s="4">
+        <v>0</v>
+      </c>
+      <c r="F65" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G65" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>43832</v>
+      </c>
+      <c r="B66" s="4">
+        <v>0</v>
+      </c>
+      <c r="F66" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G66" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>43833</v>
+      </c>
+      <c r="B67" s="4">
+        <v>0</v>
+      </c>
+      <c r="F67" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G67" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
+        <v>43834</v>
+      </c>
+      <c r="B68" s="4">
+        <v>0</v>
+      </c>
+      <c r="F68" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G68" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
+        <v>43835</v>
+      </c>
+      <c r="B69" s="4">
+        <v>0</v>
+      </c>
+      <c r="F69" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G69" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <v>43836</v>
+      </c>
+      <c r="B70" s="4">
+        <v>0</v>
+      </c>
+      <c r="F70" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G70" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <v>43837</v>
+      </c>
+      <c r="B71" s="4">
+        <v>0</v>
+      </c>
+      <c r="F71" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G71" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <v>43838</v>
+      </c>
+      <c r="B72" s="4">
+        <v>0</v>
+      </c>
+      <c r="F72" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G72" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
+        <v>43839</v>
+      </c>
+      <c r="B73" s="4">
+        <v>0</v>
+      </c>
+      <c r="F73" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G73" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="3">
+        <v>43840</v>
+      </c>
+      <c r="B74" s="4">
+        <v>0</v>
+      </c>
+      <c r="F74" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G74" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
+        <v>43841</v>
+      </c>
+      <c r="B75" s="4">
+        <v>0</v>
+      </c>
+      <c r="F75" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G75" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
+        <v>43842</v>
+      </c>
+      <c r="B76" s="4">
+        <v>0</v>
+      </c>
+      <c r="F76" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G76" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="3">
+        <v>43843</v>
+      </c>
+      <c r="B77" s="4">
+        <v>0</v>
+      </c>
+      <c r="F77" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G77" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
+        <v>43844</v>
+      </c>
+      <c r="B78" s="4">
+        <v>0</v>
+      </c>
+      <c r="F78" s="5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="G78" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="A32:H32"/>
+    <mergeCell ref="A49:H49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>